<commit_message>
[IMP] Add possibility of having non-technical descriptive header in addition to technical name header in imports and imports Set default state of patterned import export as "pending" instead of "fail"
</commit_message>
<xml_diff>
--- a/pattern_import_export_xlsx/tests/fixtures/example.partners.ok.xlsx
+++ b/pattern_import_export_xlsx/tests/fixtures/example.partners.ok.xlsx
@@ -242,17 +242,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
+      <selection pane="topLeft" activeCell="F11" activeCellId="0" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="32.8"/>

</xml_diff>